<commit_message>
Update lci files to match markets creation
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-graphite.xlsx
+++ b/premise/data/additional_inventories/lci-graphite.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\premise\premise\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EFE6D1-7BDB-7A4B-96C6-37422E356732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1420" windowWidth="30240" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1425" windowWidth="30240" windowHeight="16320"/>
   </bookViews>
   <sheets>
     <sheet name="graphite" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">graphite!$A$1:$H$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">graphite!$A$1:$H$126</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="162">
   <si>
     <t>Activity</t>
   </si>
@@ -512,12 +511,24 @@
   </si>
   <si>
     <t>ca. 90% of energy for vaccuum distillation is from coking gas.</t>
+  </si>
+  <si>
+    <t>Market created to facilitate the regionalization</t>
+  </si>
+  <si>
+    <t>Graphite</t>
+  </si>
+  <si>
+    <t>Added in the metals branch to account for metal depletion - Same quantity as original ecoinvent dataset on graphite production</t>
+  </si>
+  <si>
+    <t>market for graphite ore, mined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -610,8 +621,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{0E23583C-AEE8-A14E-BBED-EFF8448F4281}"/>
-    <cellStyle name="Per cent 2" xfId="2" xr:uid="{D55BF8F8-B642-CC4D-B89F-8E3060549780}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Per cent 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -888,22 +899,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H213"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.5" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
@@ -911,10 +922,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +933,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -930,7 +941,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -938,7 +949,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -946,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -954,7 +965,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -962,13 +973,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -1014,7 +1025,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -1037,7 +1048,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -1060,7 +1071,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -1084,7 +1095,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -1108,7 +1119,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1127,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>1</v>
       </c>
@@ -1124,7 +1135,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -1140,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
@@ -1148,7 +1159,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
@@ -1164,13 +1175,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
@@ -1196,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>142</v>
       </c>
@@ -1216,7 +1227,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>22</v>
       </c>
@@ -1240,7 +1251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>22</v>
       </c>
@@ -1264,7 +1275,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1299,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>38</v>
       </c>
@@ -1336,7 +1347,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>51</v>
       </c>
@@ -1360,7 +1371,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>54</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>27</v>
       </c>
@@ -1405,7 +1416,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>40</v>
       </c>
@@ -1426,10 +1437,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
@@ -1437,7 +1448,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>1</v>
       </c>
@@ -1445,7 +1456,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>2</v>
       </c>
@@ -1453,7 +1464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>4</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1480,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>6</v>
       </c>
@@ -1477,7 +1488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>8</v>
       </c>
@@ -1485,13 +1496,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>10</v>
       </c>
@@ -1517,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>51</v>
       </c>
@@ -1537,7 +1548,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>18</v>
       </c>
@@ -1561,7 +1572,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>47</v>
       </c>
@@ -1585,7 +1596,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>60</v>
       </c>
@@ -1609,7 +1620,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>63</v>
       </c>
@@ -1633,7 +1644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>36</v>
       </c>
@@ -1657,7 +1668,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>67</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>71</v>
       </c>
@@ -1729,7 +1740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>22</v>
       </c>
@@ -1753,7 +1764,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>75</v>
       </c>
@@ -1774,7 +1785,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>27</v>
       </c>
@@ -1795,7 +1806,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>30</v>
       </c>
@@ -1816,7 +1827,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>33</v>
       </c>
@@ -1837,10 +1848,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>0</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>1</v>
       </c>
@@ -1856,7 +1867,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>2</v>
       </c>
@@ -1864,7 +1875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>8</v>
       </c>
@@ -1896,13 +1907,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B68" s="7"/>
     </row>
-    <row r="69" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>10</v>
       </c>
@@ -1928,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>75</v>
       </c>
@@ -1948,7 +1959,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>18</v>
       </c>
@@ -1972,7 +1983,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>47</v>
       </c>
@@ -1996,7 +2007,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>80</v>
       </c>
@@ -2020,10 +2031,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2042,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>1</v>
       </c>
@@ -2039,7 +2050,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>2</v>
       </c>
@@ -2047,7 +2058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>4</v>
       </c>
@@ -2055,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>5</v>
       </c>
@@ -2063,7 +2074,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>6</v>
       </c>
@@ -2071,7 +2082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>8</v>
       </c>
@@ -2079,13 +2090,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="7"/>
     </row>
-    <row r="83" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>10</v>
       </c>
@@ -2111,7 +2122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>80</v>
       </c>
@@ -2131,7 +2142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>18</v>
       </c>
@@ -2155,7 +2166,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>47</v>
       </c>
@@ -2179,7 +2190,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>85</v>
       </c>
@@ -2203,9 +2214,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="B88" s="7">
         <f>9590/1000</f>
@@ -2215,7 +2226,7 @@
         <v>7</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>14</v>
@@ -2227,7 +2238,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>91</v>
       </c>
@@ -2251,7 +2262,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>15</v>
       </c>
@@ -2275,7 +2286,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>27</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>30</v>
       </c>
@@ -2317,7 +2328,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>33</v>
       </c>
@@ -2341,7 +2352,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>96</v>
       </c>
@@ -2362,7 +2373,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>22</v>
       </c>
@@ -2386,34 +2397,34 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7"/>
     </row>
-    <row r="97" spans="1:8" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>4</v>
       </c>
@@ -2421,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>5</v>
       </c>
@@ -2429,7 +2440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>6</v>
       </c>
@@ -2437,21 +2448,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="7"/>
+    </row>
+    <row r="104" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B104" s="7"/>
     </row>
-    <row r="105" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>10</v>
       </c>
@@ -2476,10 +2485,12 @@
       <c r="H105" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
+    </row>
+    <row r="106" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="B106" s="7">
         <v>1</v>
@@ -2488,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>13</v>
@@ -2497,1500 +2508,1654 @@
         <v>89</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B107" s="7">
+        <v>1</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="7"/>
+    </row>
+    <row r="109" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="7"/>
+    </row>
+    <row r="110" spans="1:10" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" s="7"/>
+    </row>
+    <row r="118" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B119" s="7">
+        <v>1</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B107" s="7">
+      <c r="B120" s="7">
         <f>8.7/1000</f>
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C120" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E107" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G107" s="6" t="s">
+      <c r="E120" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G120" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H107" s="6" t="s">
+      <c r="H120" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="6" t="s">
+    <row r="121" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B108" s="7">
+      <c r="B121" s="7">
         <f>2.241*43.4/1000</f>
         <v>9.7259399999999996E-2</v>
       </c>
-      <c r="C108" s="6" t="s">
+      <c r="C121" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E108" s="6" t="s">
+      <c r="E121" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F108" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G108" s="6" t="s">
+      <c r="F121" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G121" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H108" s="6" t="s">
+      <c r="H121" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="6" t="s">
+    <row r="122" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B109" s="7">
+      <c r="B122" s="7">
         <f>0.248/1000</f>
         <v>2.4800000000000001E-4</v>
       </c>
-      <c r="C109" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E109" s="6" t="s">
+      <c r="C122" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E122" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F109" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G109" s="6" t="s">
+      <c r="F122" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G122" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H109" s="6" t="s">
+      <c r="H122" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="110" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
+    <row r="123" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B110" s="7">
+      <c r="B123" s="7">
         <f>0.04/1000</f>
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="C110" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" s="6" t="s">
+      <c r="C123" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F110" s="6" t="s">
+      <c r="F123" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H110" s="6" t="s">
+      <c r="H123" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="111" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="6" t="s">
+    <row r="124" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B111" s="7">
+      <c r="B124" s="7">
         <f>0.113/1000/1000</f>
         <v>1.1300000000000001E-7</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="C124" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D111" s="6" t="s">
+      <c r="D124" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F111" s="6" t="s">
+      <c r="F124" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H111" s="6" t="s">
+      <c r="H124" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
+    <row r="125" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="7">
+      <c r="B125" s="7">
         <f>0.138/1000</f>
         <v>1.3800000000000002E-4</v>
       </c>
-      <c r="C112" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="6" t="s">
+      <c r="C125" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F112" s="6" t="s">
+      <c r="F125" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H112" s="6" t="s">
+      <c r="H125" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="6" t="s">
+    <row r="126" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B113" s="7">
+      <c r="B126" s="7">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D113" s="6" t="s">
+      <c r="C126" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F113" s="6" t="s">
+      <c r="F126" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H113" s="6" t="s">
+      <c r="H126" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:8" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
+    <row r="127" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B127" s="6">
+        <v>1.0526005961878699</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H127" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="10" t="s">
+      <c r="B129" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B116" s="11" t="s">
+    <row r="130" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B130" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="11" t="s">
+    <row r="131" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="11" t="s">
+      <c r="B131" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B118" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="11" t="s">
+      <c r="B132" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="B133" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="120" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="11" t="s">
+    <row r="134" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B120" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="11" t="s">
+      <c r="B134" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B135" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="12" t="s">
+    <row r="136" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="12" t="s">
+    <row r="137" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B137" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C123" s="12" t="s">
+      <c r="C137" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="12" t="s">
+      <c r="D137" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E123" s="12" t="s">
+      <c r="E137" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F123" s="12" t="s">
+      <c r="F137" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G123" s="12" t="s">
+      <c r="G137" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H123" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="11" t="s">
+      <c r="H137" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B124" s="11">
-        <v>1</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F124" s="11" t="s">
+      <c r="B138" s="11">
+        <v>1</v>
+      </c>
+      <c r="C138" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F138" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G124" s="11" t="s">
+      <c r="G138" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H124" s="11" t="s">
+      <c r="H138" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="11" t="s">
+    <row r="139" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B125" s="13">
+      <c r="B139" s="13">
         <f>1000/24</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="C125" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E125" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F125" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" s="11" t="s">
+      <c r="C139" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E139" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F139" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G139" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="H125" s="11" t="s">
+      <c r="H139" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="11" t="s">
+    <row r="140" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B126" s="13">
+      <c r="B140" s="13">
         <f>(4200/3.6*0.03)/24</f>
         <v>1.4583333333333333</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C140" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E126" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F126" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G126" s="11" t="s">
+      <c r="E140" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F140" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G140" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H126" s="11" t="s">
+      <c r="H140" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="11" t="s">
+    <row r="141" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B127" s="13">
+      <c r="B141" s="13">
         <f>(4200*0.97)/24</f>
         <v>169.75</v>
       </c>
-      <c r="C127" s="11" t="s">
+      <c r="C141" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E127" s="11" t="s">
+      <c r="E141" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F127" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G127" s="11" t="s">
+      <c r="F141" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G141" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="11" t="s">
+    <row r="142" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B128" s="13">
+      <c r="B142" s="13">
         <f>300/24</f>
         <v>12.5</v>
       </c>
-      <c r="C128" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D128" s="11" t="s">
+      <c r="C142" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F128" s="11" t="s">
+      <c r="F142" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="11" t="s">
+    <row r="143" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B129" s="14">
+      <c r="B143" s="14">
         <f>AVERAGE(0.025,0.846)/24</f>
         <v>1.8145833333333333E-2</v>
       </c>
-      <c r="C129" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D129" s="11" t="s">
+      <c r="C143" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F129" s="11" t="s">
+      <c r="F143" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="11" t="s">
+    <row r="144" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B130" s="14">
+      <c r="B144" s="14">
         <f>AVERAGE(0.022,0.155)/24</f>
         <v>3.6874999999999998E-3</v>
       </c>
-      <c r="C130" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D130" s="11" t="s">
+      <c r="C144" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F130" s="11" t="s">
+      <c r="F144" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="11" t="s">
+    <row r="145" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B131" s="14">
+      <c r="B145" s="14">
         <f>AVERAGE(0.026,0.821)/24</f>
         <v>1.7645833333333333E-2</v>
       </c>
-      <c r="C131" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D131" s="11" t="s">
+      <c r="C145" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F131" s="11" t="s">
+      <c r="F145" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="133" spans="1:8" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="10" t="s">
+    <row r="146" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="B147" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="134" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B134" s="11" t="s">
+    <row r="148" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B148" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="11" t="s">
+    <row r="149" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="11" t="s">
+      <c r="B149" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B136" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
+      <c r="B150" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B137" s="11" t="s">
+      <c r="B151" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="11" t="s">
+    <row r="152" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="11" t="s">
+      <c r="B152" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B139" s="11" t="s">
+      <c r="B153" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="12" t="s">
+    <row r="154" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="12" t="s">
+    <row r="155" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B141" s="12" t="s">
+      <c r="B155" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C141" s="12" t="s">
+      <c r="C155" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D141" s="12" t="s">
+      <c r="D155" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E141" s="12" t="s">
+      <c r="E155" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F141" s="12" t="s">
+      <c r="F155" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G141" s="12" t="s">
+      <c r="G155" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H141" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="11" t="s">
+      <c r="H155" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B142" s="11">
-        <v>1</v>
-      </c>
-      <c r="C142" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E142" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F142" s="11" t="s">
+      <c r="B156" s="11">
+        <v>1</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F156" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G142" s="11" t="s">
+      <c r="G156" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="11" t="s">
+    <row r="157" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B143" s="11">
-        <v>1</v>
-      </c>
-      <c r="C143" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D143" s="11" t="s">
+      <c r="B157" s="11">
+        <v>1</v>
+      </c>
+      <c r="C157" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F143" s="11" t="s">
+      <c r="F157" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="11" t="s">
+    <row r="158" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B144" s="11">
+      <c r="B158" s="11">
         <f>0.937*0.085</f>
         <v>7.9645000000000007E-2</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C158" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E144" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F144" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G144" s="11" t="s">
+      <c r="E158" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F158" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G158" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="11" t="s">
+    <row r="159" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B145" s="11">
+      <c r="B159" s="11">
         <f>0.937*3.6*0.07</f>
         <v>0.23612400000000003</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C159" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E145" s="11" t="s">
+      <c r="E159" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F145" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G145" s="11" t="s">
+      <c r="F159" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G159" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="146" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="11" t="s">
+    <row r="160" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B146" s="11">
+      <c r="B160" s="11">
         <f>0.937*3.6*0.845</f>
         <v>2.8503540000000003</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C160" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E146" s="11" t="s">
+      <c r="E160" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F146" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G146" s="11" t="s">
+      <c r="F160" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G160" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="148" spans="1:8" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="10" t="s">
+    <row r="161" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B162" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="149" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B149" s="11" t="s">
+    <row r="163" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="150" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="11" t="s">
+    <row r="164" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B150" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="11" t="s">
+      <c r="B164" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B151" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="11" t="s">
+      <c r="B165" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B152" s="11" t="s">
+      <c r="B166" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="153" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="11" t="s">
+    <row r="167" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B153" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="11" t="s">
+      <c r="B167" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B154" s="11" t="s">
+      <c r="B168" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="155" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="12" t="s">
+    <row r="169" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="12" t="s">
+    <row r="170" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B156" s="12" t="s">
+      <c r="B170" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C156" s="12" t="s">
+      <c r="C170" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D156" s="12" t="s">
+      <c r="D170" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E156" s="12" t="s">
+      <c r="E170" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F156" s="12" t="s">
+      <c r="F170" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G156" s="12" t="s">
+      <c r="G170" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H156" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="11" t="s">
+      <c r="H170" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B157" s="11">
-        <v>1</v>
-      </c>
-      <c r="C157" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E157" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F157" s="11" t="s">
+      <c r="B171" s="11">
+        <v>1</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E171" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F171" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G157" s="11" t="s">
+      <c r="G171" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="158" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="11" t="s">
+    <row r="172" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B158" s="13">
+      <c r="B172" s="13">
         <f>1/0.025</f>
         <v>40</v>
       </c>
-      <c r="C158" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E158" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F158" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G158" s="11" t="s">
+      <c r="C172" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E172" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F172" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G172" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="11" t="s">
+    <row r="173" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B159" s="13">
+      <c r="B173" s="13">
         <f>0.249*0.1/0.025</f>
         <v>0.996</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C173" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E159" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F159" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G159" s="11" t="s">
+      <c r="E173" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G173" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H159" s="11" t="s">
+      <c r="H173" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="11" t="s">
+    <row r="174" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B160" s="13">
+      <c r="B174" s="13">
         <f>(0.249*0.9*3.6)/0.025</f>
         <v>32.270400000000002</v>
       </c>
-      <c r="C160" s="11" t="s">
+      <c r="C174" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E160" s="11" t="s">
+      <c r="E174" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F160" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G160" s="11" t="s">
+      <c r="F174" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G174" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H160" s="11" t="s">
+      <c r="H174" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="11" t="s">
+    <row r="175" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B161" s="13">
+      <c r="B175" s="13">
         <f>(0.146*0.1)/0.025</f>
         <v>0.58399999999999996</v>
       </c>
-      <c r="C161" s="11" t="s">
+      <c r="C175" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E161" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F161" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G161" s="11" t="s">
+      <c r="E175" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F175" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G175" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H161" s="11" t="s">
+      <c r="H175" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="11" t="s">
+    <row r="176" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B162" s="13">
+      <c r="B176" s="13">
         <f>(0.146*0.9*3.6)/0.025</f>
         <v>18.921599999999998</v>
       </c>
-      <c r="C162" s="11" t="s">
+      <c r="C176" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E162" s="11" t="s">
+      <c r="E176" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F162" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G162" s="11" t="s">
+      <c r="F176" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G176" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H162" s="11" t="s">
+      <c r="H176" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="11" t="s">
+    <row r="177" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B163" s="13">
+      <c r="B177" s="13">
         <f>(0.318*0.05)/0.025</f>
         <v>0.63600000000000001</v>
       </c>
-      <c r="C163" s="11" t="s">
+      <c r="C177" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E163" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F163" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G163" s="11" t="s">
+      <c r="E177" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F177" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G177" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H163" s="11" t="s">
+      <c r="H177" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="11" t="s">
+    <row r="178" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B164" s="13">
+      <c r="B178" s="13">
         <f>(0.318*0.95*3.6)/0.025</f>
         <v>43.502399999999994</v>
       </c>
-      <c r="C164" s="11" t="s">
+      <c r="C178" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E164" s="11" t="s">
+      <c r="E178" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F164" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G164" s="11" t="s">
+      <c r="F178" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G178" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H164" s="11" t="s">
+      <c r="H178" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="11" t="s">
+    <row r="179" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B165" s="13">
+      <c r="B179" s="13">
         <f>0.275/0.025</f>
         <v>11</v>
       </c>
-      <c r="C165" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D165" s="11" t="s">
+      <c r="C179" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F165" s="11" t="s">
+      <c r="F179" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="167" spans="1:8" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A167" s="10" t="s">
+    <row r="180" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B181" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B168" s="11" t="s">
+    <row r="182" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B182" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="11" t="s">
+    <row r="183" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B169" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="11" t="s">
+      <c r="B183" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B170" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="11" t="s">
+      <c r="B184" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B171" s="11" t="s">
+      <c r="B185" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="172" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="11" t="s">
+    <row r="186" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B172" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="11" t="s">
+      <c r="B186" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B173" s="11" t="s">
+      <c r="B187" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="174" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="12" t="s">
+    <row r="188" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="12" t="s">
+    <row r="189" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B175" s="12" t="s">
+      <c r="B189" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C175" s="12" t="s">
+      <c r="C189" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D175" s="12" t="s">
+      <c r="D189" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E175" s="12" t="s">
+      <c r="E189" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F175" s="12" t="s">
+      <c r="F189" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G175" s="12" t="s">
+      <c r="G189" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H175" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="11" t="s">
+      <c r="H189" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B176" s="11">
-        <v>1</v>
-      </c>
-      <c r="C176" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E176" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F176" s="11" t="s">
+      <c r="B190" s="11">
+        <v>1</v>
+      </c>
+      <c r="C190" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E190" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F190" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G176" s="11" t="s">
+      <c r="G190" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="177" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="11" t="s">
+    <row r="191" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B177" s="15">
+      <c r="B191" s="15">
         <v>1.3513513513513513</v>
       </c>
-      <c r="C177" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E177" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F177" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G177" s="11" t="s">
+      <c r="C191" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E191" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F191" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G191" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="11" t="s">
+    <row r="192" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B178" s="15">
+      <c r="B192" s="15">
         <f>(4.4*0.1)/0.74</f>
         <v>0.59459459459459463</v>
       </c>
-      <c r="C178" s="11" t="s">
+      <c r="C192" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E178" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F178" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G178" s="11" t="s">
+      <c r="E192" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F192" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G192" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="11" t="s">
+    <row r="193" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B179" s="15">
+      <c r="B193" s="15">
         <f>(4.4*0.9*3.6)/0.74</f>
         <v>19.264864864864869</v>
       </c>
-      <c r="C179" s="11" t="s">
+      <c r="C193" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E179" s="11" t="s">
+      <c r="E193" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F179" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G179" s="11" t="s">
+      <c r="F193" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G193" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="11" t="s">
+    <row r="194" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B180" s="15">
+      <c r="B194" s="15">
         <v>1.7567567567567569E-2</v>
       </c>
-      <c r="C180" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D180" s="11" t="s">
+      <c r="C194" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F180" s="11" t="s">
+      <c r="F194" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="181" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="11" t="s">
+    <row r="195" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B181" s="15">
+      <c r="B195" s="15">
         <v>1.891891891891892E-2</v>
       </c>
-      <c r="C181" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D181" s="11" t="s">
+      <c r="C195" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F181" s="11" t="s">
+      <c r="F195" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="11" t="s">
+    <row r="196" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B182" s="15">
+      <c r="B196" s="15">
         <v>0.20945945945945946</v>
       </c>
-      <c r="C182" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D182" s="11" t="s">
+      <c r="C196" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D196" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F182" s="11" t="s">
+      <c r="F196" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="184" spans="1:8" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A184" s="10" t="s">
+    <row r="197" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B184" s="10" t="s">
+      <c r="B198" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="185" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B185" s="11" t="s">
+    <row r="199" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B199" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="186" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="11" t="s">
+    <row r="200" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B186" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="11" t="s">
+      <c r="B200" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B187" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="11" t="s">
+      <c r="B201" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B188" s="11" t="s">
+      <c r="B202" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="189" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="11" t="s">
+    <row r="203" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B189" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="11" t="s">
+      <c r="B203" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B190" s="11" t="s">
+      <c r="B204" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="12" t="s">
+    <row r="205" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="12" t="s">
+    <row r="206" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B192" s="12" t="s">
+      <c r="B206" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C192" s="12" t="s">
+      <c r="C206" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D192" s="12" t="s">
+      <c r="D206" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E192" s="12" t="s">
+      <c r="E206" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F192" s="12" t="s">
+      <c r="F206" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G192" s="12" t="s">
+      <c r="G206" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H192" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="11" t="s">
+      <c r="H206" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B193" s="11">
-        <v>1</v>
-      </c>
-      <c r="C193" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E193" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F193" s="11" t="s">
+      <c r="B207" s="11">
+        <v>1</v>
+      </c>
+      <c r="C207" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E207" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F207" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G193" s="11" t="s">
+      <c r="G207" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="194" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="11" t="s">
+    <row r="208" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B194" s="13">
+      <c r="B208" s="13">
         <v>0.80321285140562249</v>
       </c>
-      <c r="C194" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E194" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F194" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G194" s="11" t="s">
+      <c r="C208" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E208" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F208" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G208" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="195" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="11" t="s">
+    <row r="209" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B195" s="13">
+      <c r="B209" s="13">
         <v>0.20080321285140562</v>
       </c>
-      <c r="C195" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E195" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F195" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G195" s="11" t="s">
+      <c r="C209" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E209" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F209" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G209" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="196" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="11" t="s">
+    <row r="210" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B196" s="13">
+      <c r="B210" s="13">
         <v>12.650602409638553</v>
       </c>
-      <c r="C196" s="11" t="s">
+      <c r="C210" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E196" s="11" t="s">
+      <c r="E210" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F196" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G196" s="11" t="s">
+      <c r="F210" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G210" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="11" t="s">
+    <row r="211" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B197" s="13">
+      <c r="B211" s="13">
         <v>2.6807228915662652E-3</v>
       </c>
-      <c r="C197" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D197" s="11" t="s">
+      <c r="C211" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F197" s="11" t="s">
+      <c r="F211" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="11" t="s">
+    <row r="212" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B198" s="14">
+      <c r="B212" s="14">
         <v>7.9819277108433736E-5</v>
       </c>
-      <c r="C198" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D198" s="11" t="s">
+      <c r="C212" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F198" s="11" t="s">
+      <c r="F212" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="199" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="11" t="s">
+    <row r="213" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B199" s="14">
+      <c r="B213" s="14">
         <v>2.4698795180722895E-4</v>
       </c>
-      <c r="C199" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D199" s="11" t="s">
+      <c r="C213" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F199" s="11" t="s">
+      <c r="F213" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="201" spans="1:7" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A201" s="10" t="s">
+    <row r="214" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A215" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B201" s="10" t="s">
+      <c r="B215" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="202" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B202" s="11" t="s">
+    <row r="216" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B216" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="203" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="11" t="s">
+    <row r="217" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B203" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="11" t="s">
+      <c r="B217" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B204" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="11" t="s">
+      <c r="B218" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B205" s="11" t="s">
+      <c r="B219" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="206" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="11" t="s">
+    <row r="220" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B206" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="11" t="s">
+      <c r="B220" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B207" s="11" t="s">
+      <c r="B221" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="208" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="12" t="s">
+    <row r="222" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="12" t="s">
+    <row r="223" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B209" s="12" t="s">
+      <c r="B223" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C209" s="12" t="s">
+      <c r="C223" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D209" s="12" t="s">
+      <c r="D223" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E209" s="12" t="s">
+      <c r="E223" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F209" s="12" t="s">
+      <c r="F223" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G209" s="12" t="s">
+      <c r="G223" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H209" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="11" t="s">
+      <c r="H223" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B210" s="11">
-        <v>1</v>
-      </c>
-      <c r="C210" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E210" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F210" s="11" t="s">
+      <c r="B224" s="11">
+        <v>1</v>
+      </c>
+      <c r="C224" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E224" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F224" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G210" s="11" t="s">
+      <c r="G224" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="11" t="s">
+    <row r="225" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B211" s="15">
+      <c r="B225" s="15">
         <v>1.0204081632653061</v>
       </c>
-      <c r="C211" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E211" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F211" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G211" s="11" t="s">
+      <c r="C225" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E225" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F225" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G225" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="11" t="s">
+    <row r="226" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B212" s="15">
+      <c r="B226" s="15">
         <f>(0.88*3.6)/0.98</f>
         <v>3.2326530612244899</v>
       </c>
-      <c r="C212" s="11" t="s">
+      <c r="C226" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E212" s="11" t="s">
+      <c r="E226" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F212" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G212" s="11" t="s">
+      <c r="F226" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G226" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="11" t="s">
+    <row r="227" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B213" s="15">
+      <c r="B227" s="15">
         <v>1.9693877551020408E-2</v>
       </c>
-      <c r="C213" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D213" s="11" t="s">
+      <c r="C227" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D227" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F213" s="11" t="s">
+      <c r="F227" s="11" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H113" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H127"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>